<commit_message>
Before put data on sheet confirm.
</commit_message>
<xml_diff>
--- a/CampaignTrackly/bin/Debug/Book1.xlsx
+++ b/CampaignTrackly/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R32b47f58c8c04259"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rb64a8067de9e436d"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="525" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R5680161bf1974380"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Re7bd08cdb7e341fa"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{34d2b85a-c9fa-4397-a92d-e08133cc81da}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{b7279542-6cf1-4823-8637-3f5c5e2c0121}">
   <we:reference id="936451d4-fe5c-4f6b-9d8f-621493072970" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Update login form and dialog for confirmation
</commit_message>
<xml_diff>
--- a/CampaignTrackly/bin/Debug/Book1.xlsx
+++ b/CampaignTrackly/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rb64a8067de9e436d"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rdcb4095197684a9b"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="525" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Re7bd08cdb7e341fa"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Re78f756819cd4f01"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{b7279542-6cf1-4823-8637-3f5c5e2c0121}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{9742f4ae-c968-47d0-8737-970f5786cc0f}">
   <we:reference id="936451d4-fe5c-4f6b-9d8f-621493072970" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Update Code add QR code column and fix date column
</commit_message>
<xml_diff>
--- a/CampaignTrackly/bin/Debug/Book1.xlsx
+++ b/CampaignTrackly/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rdcb4095197684a9b"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R8ae13e5c4087432c"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="525" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Re78f756819cd4f01"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R3b553599eb2041d6"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{9742f4ae-c968-47d0-8737-970f5786cc0f}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{fb9921eb-c64d-4698-92ac-efb1f18bd12f}">
   <we:reference id="936451d4-fe5c-4f6b-9d8f-621493072970" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Fix the Date Column
</commit_message>
<xml_diff>
--- a/CampaignTrackly/bin/Debug/Book1.xlsx
+++ b/CampaignTrackly/bin/Debug/Book1.xlsx
@@ -2,21 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R8ae13e5c4087432c"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rdb160e59387549ef"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="" visibility="1" width="525" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R3b553599eb2041d6"/>
+  <wetp:taskpane dockstate="" visibility="1" width="437" row="1">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Ree1a6cc9585f44a6"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{fb9921eb-c64d-4698-92ac-efb1f18bd12f}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{4dd6c075-2f98-4521-9b84-27b3ed0a99ab}">
   <we:reference id="936451d4-fe5c-4f6b-9d8f-621493072970" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Add Dropdown for Custom tag
</commit_message>
<xml_diff>
--- a/CampaignTrackly/bin/Debug/Book1.xlsx
+++ b/CampaignTrackly/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rdb160e59387549ef"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rf795a35a23114387"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="437" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Ree1a6cc9585f44a6"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R9bf1b09b768d4cbe"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{4dd6c075-2f98-4521-9b84-27b3ed0a99ab}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{9b952cf7-e2fe-4235-8934-9f047fd62204}">
   <we:reference id="936451d4-fe5c-4f6b-9d8f-621493072970" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Fix Drodown data issue
</commit_message>
<xml_diff>
--- a/CampaignTrackly/bin/Debug/Book1.xlsx
+++ b/CampaignTrackly/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rf795a35a23114387"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R062167aab05a4509"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="437" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R9bf1b09b768d4cbe"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R62c8066c516247e6"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{9b952cf7-e2fe-4235-8934-9f047fd62204}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{f7e493cc-0797-41bf-a8cc-4de9fe831bfb}">
   <we:reference id="936451d4-fe5c-4f6b-9d8f-621493072970" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Fix Dropdown and Manual entry
</commit_message>
<xml_diff>
--- a/CampaignTrackly/bin/Debug/Book1.xlsx
+++ b/CampaignTrackly/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R062167aab05a4509"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R51b9637b2b4a4391"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="437" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R62c8066c516247e6"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Rd01b92b8fd374b82"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{f7e493cc-0797-41bf-a8cc-4de9fe831bfb}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{917c6db5-0adf-4960-9500-87f9e8ed6934}">
   <we:reference id="936451d4-fe5c-4f6b-9d8f-621493072970" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Fix Custom Tag issue
</commit_message>
<xml_diff>
--- a/CampaignTrackly/bin/Debug/Book1.xlsx
+++ b/CampaignTrackly/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R76fbd206af694bc6"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R1018afadcbd1491c"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="437" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R8112f774b9f84a7c"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Re4374f57d80242aa"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{06f69763-11e6-44b0-9d13-516d7abaac59}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{1177c1a1-bfe6-4dad-b782-c8476e10676a}">
   <we:reference id="936451d4-fe5c-4f6b-9d8f-621493072970" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Fix issue of dropdown
</commit_message>
<xml_diff>
--- a/CampaignTrackly/bin/Debug/Book1.xlsx
+++ b/CampaignTrackly/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R1018afadcbd1491c"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R8dcdfeea1ee44393"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="437" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Re4374f57d80242aa"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R295e12ef2d5a48ec"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{1177c1a1-bfe6-4dad-b782-c8476e10676a}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{c78dfda1-323b-47ac-826d-c8350ac19ee5}">
   <we:reference id="936451d4-fe5c-4f6b-9d8f-621493072970" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
dropdown for existing campaign
</commit_message>
<xml_diff>
--- a/CampaignTrackly/bin/Debug/Book1.xlsx
+++ b/CampaignTrackly/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R75713b99a3ed41e7"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R932003c6422442b9"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="437" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R8ddc368accb14970"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R3f92e558cf244101"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{b0067db1-b269-476d-a109-bd6075fb6923}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{46855c17-ffdb-48f6-bd9c-f00d6076a4c6}">
   <we:reference id="936451d4-fe5c-4f6b-9d8f-621493072970" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
generating campaign name with tags
</commit_message>
<xml_diff>
--- a/CampaignTrackly/bin/Debug/Book1.xlsx
+++ b/CampaignTrackly/bin/Debug/Book1.xlsx
@@ -2,21 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R932003c6422442b9"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Re03d42a27d0e48e3"/>
   </x:sheets>
 </x:workbook>
 </file>
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="" visibility="1" width="437" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R3f92e558cf244101"/>
+  <wetp:taskpane dockstate="" visibility="1" width="525" row="1">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R324779e33018454c"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{46855c17-ffdb-48f6-bd9c-f00d6076a4c6}">
+<we:webextension xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{0fb59cf0-5606-4dad-b8a8-e22a817e2816}">
   <we:reference id="936451d4-fe5c-4f6b-9d8f-621493072970" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>